<commit_message>
#105 #104 Doku erweitert + gantt angepasst
</commit_message>
<xml_diff>
--- a/organisation/documentation/gantt.xlsx
+++ b/organisation/documentation/gantt.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Task</t>
   </si>
@@ -177,14 +177,20 @@
     <t>Sprint 2 (05.03.2018 - 09.05.2018)</t>
   </si>
   <si>
-    <t>Tage</t>
+    <t>Erledigt</t>
+  </si>
+  <si>
+    <t>Geplant</t>
+  </si>
+  <si>
+    <t>Dauer [Tage]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,8 +282,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,8 +357,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -561,6 +587,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -658,7 +721,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -677,38 +740,50 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="34">
     <cellStyle name="% abgeschlossen" xfId="17"/>
     <cellStyle name="Aktivität" xfId="3"/>
     <cellStyle name="Bezeichnung" xfId="6"/>
-    <cellStyle name="Erklärender Text 2" xfId="13" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text 3" xfId="29" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text 4" xfId="33" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text 2" xfId="13"/>
+    <cellStyle name="Erklärender Text 3" xfId="29"/>
+    <cellStyle name="Erklärender Text 4" xfId="33"/>
     <cellStyle name="Legende &quot;Tatsächlich&quot;" xfId="16"/>
     <cellStyle name="Legende zu &quot;% abgeschlossen (hinter dem Plan)&quot;" xfId="19"/>
     <cellStyle name="Legende zu &quot;tatsächlich (hinter dem Plan)&quot;" xfId="18"/>
@@ -716,25 +791,25 @@
     <cellStyle name="Projektüberschriften" xfId="5"/>
     <cellStyle name="Prozent abgeschlossen" xfId="7"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" customBuiltin="1"/>
-    <cellStyle name="Standard 3" xfId="20" customBuiltin="1"/>
-    <cellStyle name="Standard 4" xfId="30" customBuiltin="1"/>
+    <cellStyle name="Standard 2" xfId="1"/>
+    <cellStyle name="Standard 3" xfId="20"/>
+    <cellStyle name="Standard 4" xfId="30"/>
     <cellStyle name="Steuerelement zum Hervorheben von Zeiträumen" xfId="8"/>
-    <cellStyle name="Überschrift 1 2" xfId="2" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1 3" xfId="21" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1 4" xfId="23" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2 2" xfId="10" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2 3" xfId="26" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2 4" xfId="24" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3 2" xfId="11" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3 3" xfId="27" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3 4" xfId="22" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4 2" xfId="12" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4 3" xfId="28" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4 4" xfId="32" customBuiltin="1"/>
-    <cellStyle name="Überschrift 5" xfId="9" customBuiltin="1"/>
-    <cellStyle name="Überschrift 6" xfId="25" customBuiltin="1"/>
-    <cellStyle name="Überschrift 7" xfId="31" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1 2" xfId="2"/>
+    <cellStyle name="Überschrift 1 3" xfId="21"/>
+    <cellStyle name="Überschrift 1 4" xfId="23"/>
+    <cellStyle name="Überschrift 2 2" xfId="10"/>
+    <cellStyle name="Überschrift 2 3" xfId="26"/>
+    <cellStyle name="Überschrift 2 4" xfId="24"/>
+    <cellStyle name="Überschrift 3 2" xfId="11"/>
+    <cellStyle name="Überschrift 3 3" xfId="27"/>
+    <cellStyle name="Überschrift 3 4" xfId="22"/>
+    <cellStyle name="Überschrift 4 2" xfId="12"/>
+    <cellStyle name="Überschrift 4 3" xfId="28"/>
+    <cellStyle name="Überschrift 4 4" xfId="32"/>
+    <cellStyle name="Überschrift 5" xfId="9"/>
+    <cellStyle name="Überschrift 6" xfId="25"/>
+    <cellStyle name="Überschrift 7" xfId="31"/>
     <cellStyle name="Überschriften für Zeiträume" xfId="4"/>
     <cellStyle name="Zeitraumwert" xfId="14"/>
   </cellStyles>
@@ -1028,172 +1103,181 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:AB57"/>
+  <dimension ref="B2:AA58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA56" sqref="B2:AA56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="68.7109375" customWidth="1"/>
-    <col min="3" max="27" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="54.5703125" customWidth="1"/>
+    <col min="3" max="27" width="2.7109375" customWidth="1"/>
+    <col min="28" max="28" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:28">
+    <row r="2" spans="2:27">
       <c r="C2" s="2"/>
+      <c r="D2" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="3"/>
-    </row>
-    <row r="4" spans="2:28">
-      <c r="C4" s="14" t="s">
+      <c r="I2" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+    </row>
+    <row r="4" spans="2:27">
+      <c r="C4" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="15" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
-    </row>
-    <row r="5" spans="2:28" ht="21">
-      <c r="B5" s="18" t="s">
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+    </row>
+    <row r="5" spans="2:27">
+      <c r="C5" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+      <c r="Q5" s="27"/>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27"/>
+      <c r="U5" s="27"/>
+      <c r="V5" s="27"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="27"/>
+      <c r="Z5" s="27"/>
+      <c r="AA5" s="28"/>
+    </row>
+    <row r="6" spans="2:27" ht="21">
+      <c r="B6" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>2</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E6" s="4">
         <v>3</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F6" s="4">
         <v>4</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G6" s="4">
         <v>5</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H6" s="4">
         <v>6</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I6" s="4">
         <v>7</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J6" s="4">
         <v>8</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K6" s="4">
         <v>9</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L6" s="4">
         <v>10</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M6" s="4">
         <v>11</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N6" s="4">
         <v>12</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O6" s="4">
         <v>13</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P6" s="4">
         <v>14</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q6" s="4">
         <v>15</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R6" s="4">
         <v>16</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S6" s="4">
         <v>17</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T6" s="4">
         <v>18</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U6" s="4">
         <v>19</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V6" s="4">
         <v>20</v>
       </c>
-      <c r="W5" s="4">
+      <c r="W6" s="4">
         <v>21</v>
       </c>
-      <c r="X5" s="4">
+      <c r="X6" s="4">
         <v>22</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Y6" s="4">
         <v>23</v>
       </c>
-      <c r="Z5" s="4">
+      <c r="Z6" s="4">
         <v>24</v>
       </c>
-      <c r="AA5" s="4">
+      <c r="AA6" s="4">
         <v>25</v>
       </c>
-      <c r="AB5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="2:28">
-      <c r="B6" s="19" t="s">
+    </row>
+    <row r="7" spans="2:27" ht="18" customHeight="1">
+      <c r="B7" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="8"/>
-    </row>
-    <row r="7" spans="2:28">
-      <c r="B7" s="20" t="s">
-        <v>2</v>
-      </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -1201,8 +1285,8 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="16"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="14"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
@@ -1218,12 +1302,12 @@
       <c r="Z7" s="7"/>
       <c r="AA7" s="8"/>
     </row>
-    <row r="8" spans="2:28">
-      <c r="B8" s="20" t="s">
-        <v>3</v>
+    <row r="8" spans="2:27" ht="18" customHeight="1">
+      <c r="B8" s="32" t="s">
+        <v>2</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -1232,7 +1316,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="8"/>
-      <c r="M8" s="16"/>
+      <c r="M8" s="14"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
@@ -1248,11 +1332,11 @@
       <c r="Z8" s="7"/>
       <c r="AA8" s="8"/>
     </row>
-    <row r="9" spans="2:28">
-      <c r="B9" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="9"/>
+    <row r="9" spans="2:27" ht="18" customHeight="1">
+      <c r="B9" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6"/>
       <c r="D9" s="10"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -1262,7 +1346,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="8"/>
-      <c r="M9" s="16"/>
+      <c r="M9" s="14"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -1278,13 +1362,13 @@
       <c r="Z9" s="7"/>
       <c r="AA9" s="8"/>
     </row>
-    <row r="10" spans="2:28">
-      <c r="B10" s="20" t="s">
-        <v>5</v>
+    <row r="10" spans="2:27" ht="18" customHeight="1">
+      <c r="B10" s="32" t="s">
+        <v>4</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
@@ -1292,7 +1376,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="8"/>
-      <c r="M10" s="16"/>
+      <c r="M10" s="14"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
@@ -1308,13 +1392,13 @@
       <c r="Z10" s="7"/>
       <c r="AA10" s="8"/>
     </row>
-    <row r="11" spans="2:28">
-      <c r="B11" s="20" t="s">
-        <v>6</v>
+    <row r="11" spans="2:27" ht="18" customHeight="1">
+      <c r="B11" s="32" t="s">
+        <v>5</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
@@ -1322,7 +1406,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="8"/>
-      <c r="M11" s="16"/>
+      <c r="M11" s="14"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
@@ -1338,13 +1422,13 @@
       <c r="Z11" s="7"/>
       <c r="AA11" s="8"/>
     </row>
-    <row r="12" spans="2:28">
-      <c r="B12" s="20" t="s">
-        <v>7</v>
+    <row r="12" spans="2:27" ht="18" customHeight="1">
+      <c r="B12" s="32" t="s">
+        <v>6</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -1352,7 +1436,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="8"/>
-      <c r="M12" s="16"/>
+      <c r="M12" s="14"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
@@ -1368,21 +1452,21 @@
       <c r="Z12" s="7"/>
       <c r="AA12" s="8"/>
     </row>
-    <row r="13" spans="2:28">
-      <c r="B13" s="20" t="s">
-        <v>8</v>
+    <row r="13" spans="2:27" ht="18" customHeight="1">
+      <c r="B13" s="32" t="s">
+        <v>7</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="8"/>
-      <c r="M13" s="16"/>
+      <c r="M13" s="14"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
@@ -1398,21 +1482,21 @@
       <c r="Z13" s="7"/>
       <c r="AA13" s="8"/>
     </row>
-    <row r="14" spans="2:28">
-      <c r="B14" s="20" t="s">
-        <v>9</v>
+    <row r="14" spans="2:27" ht="18" customHeight="1">
+      <c r="B14" s="32" t="s">
+        <v>8</v>
       </c>
       <c r="C14" s="9"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="8"/>
-      <c r="M14" s="16"/>
+      <c r="M14" s="14"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
@@ -1428,21 +1512,21 @@
       <c r="Z14" s="7"/>
       <c r="AA14" s="8"/>
     </row>
-    <row r="15" spans="2:28">
-      <c r="B15" s="20" t="s">
-        <v>10</v>
+    <row r="15" spans="2:27" ht="18" customHeight="1">
+      <c r="B15" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="7"/>
+      <c r="J15" s="10"/>
       <c r="K15" s="7"/>
       <c r="L15" s="8"/>
-      <c r="M15" s="16"/>
+      <c r="M15" s="14"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
@@ -1458,21 +1542,21 @@
       <c r="Z15" s="7"/>
       <c r="AA15" s="8"/>
     </row>
-    <row r="16" spans="2:28">
-      <c r="B16" s="20" t="s">
-        <v>11</v>
+    <row r="16" spans="2:27" ht="18" customHeight="1">
+      <c r="B16" s="32" t="s">
+        <v>10</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="8"/>
-      <c r="M16" s="16"/>
+      <c r="M16" s="14"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
@@ -1488,9 +1572,9 @@
       <c r="Z16" s="7"/>
       <c r="AA16" s="8"/>
     </row>
-    <row r="17" spans="2:27">
-      <c r="B17" s="20" t="s">
-        <v>12</v>
+    <row r="17" spans="2:27" ht="18" customHeight="1">
+      <c r="B17" s="32" t="s">
+        <v>11</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="7"/>
@@ -1502,7 +1586,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="8"/>
-      <c r="M17" s="16"/>
+      <c r="M17" s="14"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
@@ -1518,9 +1602,9 @@
       <c r="Z17" s="7"/>
       <c r="AA17" s="8"/>
     </row>
-    <row r="18" spans="2:27">
-      <c r="B18" s="20" t="s">
-        <v>13</v>
+    <row r="18" spans="2:27" ht="18" customHeight="1">
+      <c r="B18" s="32" t="s">
+        <v>12</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="7"/>
@@ -1528,12 +1612,12 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
@@ -1548,9 +1632,9 @@
       <c r="Z18" s="7"/>
       <c r="AA18" s="8"/>
     </row>
-    <row r="19" spans="2:27">
-      <c r="B19" s="20" t="s">
-        <v>14</v>
+    <row r="19" spans="2:27" ht="18" customHeight="1">
+      <c r="B19" s="32" t="s">
+        <v>13</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="7"/>
@@ -1561,9 +1645,9 @@
       <c r="I19" s="7"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="7"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="10"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
@@ -1578,9 +1662,9 @@
       <c r="Z19" s="7"/>
       <c r="AA19" s="8"/>
     </row>
-    <row r="20" spans="2:27">
-      <c r="B20" s="20" t="s">
-        <v>15</v>
+    <row r="20" spans="2:27" ht="18" customHeight="1">
+      <c r="B20" s="32" t="s">
+        <v>14</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="7"/>
@@ -1588,11 +1672,11 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
-      <c r="I20" s="10"/>
+      <c r="I20" s="7"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="L20" s="8"/>
-      <c r="M20" s="16"/>
+      <c r="M20" s="14"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
@@ -1608,21 +1692,21 @@
       <c r="Z20" s="7"/>
       <c r="AA20" s="8"/>
     </row>
-    <row r="21" spans="2:27">
-      <c r="B21" s="20" t="s">
-        <v>16</v>
+    <row r="21" spans="2:27" ht="18" customHeight="1">
+      <c r="B21" s="32" t="s">
+        <v>15</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="10"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="7"/>
+      <c r="K21" s="10"/>
       <c r="L21" s="8"/>
-      <c r="M21" s="16"/>
+      <c r="M21" s="14"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
@@ -1638,21 +1722,21 @@
       <c r="Z21" s="7"/>
       <c r="AA21" s="8"/>
     </row>
-    <row r="22" spans="2:27">
-      <c r="B22" s="20" t="s">
-        <v>17</v>
+    <row r="22" spans="2:27" ht="18" customHeight="1">
+      <c r="B22" s="32" t="s">
+        <v>16</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="7"/>
       <c r="L22" s="8"/>
-      <c r="M22" s="16"/>
+      <c r="M22" s="14"/>
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
@@ -1668,21 +1752,21 @@
       <c r="Z22" s="7"/>
       <c r="AA22" s="8"/>
     </row>
-    <row r="23" spans="2:27">
-      <c r="B23" s="20" t="s">
-        <v>18</v>
+    <row r="23" spans="2:27" ht="18" customHeight="1">
+      <c r="B23" s="32" t="s">
+        <v>17</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
+      <c r="J23" s="10"/>
       <c r="K23" s="7"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="16"/>
+      <c r="M23" s="14"/>
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
@@ -1698,21 +1782,21 @@
       <c r="Z23" s="7"/>
       <c r="AA23" s="8"/>
     </row>
-    <row r="24" spans="2:27">
-      <c r="B24" s="20" t="s">
-        <v>19</v>
+    <row r="24" spans="2:27" ht="18" customHeight="1">
+      <c r="B24" s="32" t="s">
+        <v>18</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
+      <c r="G24" s="10"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
       <c r="K24" s="7"/>
       <c r="L24" s="8"/>
-      <c r="M24" s="16"/>
+      <c r="M24" s="14"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
@@ -1728,21 +1812,21 @@
       <c r="Z24" s="7"/>
       <c r="AA24" s="8"/>
     </row>
-    <row r="25" spans="2:27">
-      <c r="B25" s="20" t="s">
-        <v>20</v>
+    <row r="25" spans="2:27" ht="18" customHeight="1">
+      <c r="B25" s="32" t="s">
+        <v>19</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="7"/>
       <c r="L25" s="8"/>
-      <c r="M25" s="16"/>
+      <c r="M25" s="14"/>
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
@@ -1758,9 +1842,9 @@
       <c r="Z25" s="7"/>
       <c r="AA25" s="8"/>
     </row>
-    <row r="26" spans="2:27">
-      <c r="B26" s="20" t="s">
-        <v>21</v>
+    <row r="26" spans="2:27" ht="18" customHeight="1">
+      <c r="B26" s="32" t="s">
+        <v>20</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="7"/>
@@ -1769,10 +1853,10 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="16"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="14"/>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
@@ -1788,21 +1872,21 @@
       <c r="Z26" s="7"/>
       <c r="AA26" s="8"/>
     </row>
-    <row r="27" spans="2:27">
-      <c r="B27" s="20" t="s">
-        <v>22</v>
+    <row r="27" spans="2:27" ht="18" customHeight="1">
+      <c r="B27" s="32" t="s">
+        <v>21</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
       <c r="K27" s="10"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="16"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="14"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
@@ -1818,9 +1902,9 @@
       <c r="Z27" s="7"/>
       <c r="AA27" s="8"/>
     </row>
-    <row r="28" spans="2:27">
-      <c r="B28" s="20" t="s">
-        <v>23</v>
+    <row r="28" spans="2:27" ht="18" customHeight="1">
+      <c r="B28" s="32" t="s">
+        <v>22</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="7"/>
@@ -1830,9 +1914,9 @@
       <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
-      <c r="K28" s="7"/>
+      <c r="K28" s="10"/>
       <c r="L28" s="8"/>
-      <c r="M28" s="16"/>
+      <c r="M28" s="14"/>
       <c r="N28" s="7"/>
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
@@ -1848,21 +1932,21 @@
       <c r="Z28" s="7"/>
       <c r="AA28" s="8"/>
     </row>
-    <row r="29" spans="2:27">
-      <c r="B29" s="20" t="s">
-        <v>24</v>
+    <row r="29" spans="2:27" ht="18" customHeight="1">
+      <c r="B29" s="32" t="s">
+        <v>23</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
+      <c r="G29" s="10"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
+      <c r="K29" s="7"/>
       <c r="L29" s="8"/>
-      <c r="M29" s="16"/>
+      <c r="M29" s="14"/>
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
@@ -1878,29 +1962,29 @@
       <c r="Z29" s="7"/>
       <c r="AA29" s="8"/>
     </row>
-    <row r="30" spans="2:27">
-      <c r="B30" s="20" t="s">
-        <v>25</v>
+    <row r="30" spans="2:27" ht="18" customHeight="1">
+      <c r="B30" s="32" t="s">
+        <v>24</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
       <c r="L30" s="8"/>
-      <c r="M30" s="16"/>
+      <c r="M30" s="14"/>
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
-      <c r="R30" s="10"/>
-      <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="10"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
       <c r="V30" s="7"/>
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
@@ -1908,9 +1992,9 @@
       <c r="Z30" s="7"/>
       <c r="AA30" s="8"/>
     </row>
-    <row r="31" spans="2:27">
-      <c r="B31" s="20" t="s">
-        <v>26</v>
+    <row r="31" spans="2:27" ht="18" customHeight="1">
+      <c r="B31" s="32" t="s">
+        <v>25</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="7"/>
@@ -1922,15 +2006,15 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
       <c r="L31" s="8"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
       <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="7"/>
@@ -1938,9 +2022,9 @@
       <c r="Z31" s="7"/>
       <c r="AA31" s="8"/>
     </row>
-    <row r="32" spans="2:27">
-      <c r="B32" s="20" t="s">
-        <v>27</v>
+    <row r="32" spans="2:27" ht="18" customHeight="1">
+      <c r="B32" s="32" t="s">
+        <v>26</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="7"/>
@@ -1952,25 +2036,25 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
       <c r="L32" s="8"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
       <c r="Q32" s="7"/>
       <c r="R32" s="7"/>
-      <c r="S32" s="11"/>
-      <c r="T32" s="11"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="11"/>
-      <c r="Z32" s="11"/>
-      <c r="AA32" s="12"/>
-    </row>
-    <row r="33" spans="2:27">
-      <c r="B33" s="20" t="s">
-        <v>28</v>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="8"/>
+    </row>
+    <row r="33" spans="2:27" ht="18" customHeight="1">
+      <c r="B33" s="32" t="s">
+        <v>27</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="7"/>
@@ -1982,25 +2066,25 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
       <c r="L33" s="8"/>
-      <c r="M33" s="16"/>
+      <c r="M33" s="14"/>
       <c r="N33" s="7"/>
-      <c r="O33" s="10"/>
+      <c r="O33" s="7"/>
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
       <c r="R33" s="7"/>
-      <c r="S33" s="7"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="7"/>
-      <c r="V33" s="7"/>
-      <c r="W33" s="7"/>
-      <c r="X33" s="7"/>
-      <c r="Y33" s="7"/>
-      <c r="Z33" s="7"/>
-      <c r="AA33" s="8"/>
-    </row>
-    <row r="34" spans="2:27">
-      <c r="B34" s="20" t="s">
-        <v>29</v>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="10"/>
+      <c r="X33" s="10"/>
+      <c r="Y33" s="10"/>
+      <c r="Z33" s="10"/>
+      <c r="AA33" s="30"/>
+    </row>
+    <row r="34" spans="2:27" ht="18" customHeight="1">
+      <c r="B34" s="32" t="s">
+        <v>28</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="7"/>
@@ -2012,7 +2096,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
       <c r="L34" s="8"/>
-      <c r="M34" s="16"/>
+      <c r="M34" s="14"/>
       <c r="N34" s="7"/>
       <c r="O34" s="10"/>
       <c r="P34" s="7"/>
@@ -2028,9 +2112,9 @@
       <c r="Z34" s="7"/>
       <c r="AA34" s="8"/>
     </row>
-    <row r="35" spans="2:27">
-      <c r="B35" s="20" t="s">
-        <v>30</v>
+    <row r="35" spans="2:27" ht="18" customHeight="1">
+      <c r="B35" s="32" t="s">
+        <v>29</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="7"/>
@@ -2042,12 +2126,12 @@
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
       <c r="L35" s="8"/>
-      <c r="M35" s="16"/>
+      <c r="M35" s="14"/>
       <c r="N35" s="7"/>
-      <c r="O35" s="7"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
       <c r="S35" s="7"/>
       <c r="T35" s="7"/>
       <c r="U35" s="7"/>
@@ -2058,9 +2142,9 @@
       <c r="Z35" s="7"/>
       <c r="AA35" s="8"/>
     </row>
-    <row r="36" spans="2:27">
-      <c r="B36" s="20" t="s">
-        <v>31</v>
+    <row r="36" spans="2:27" ht="18" customHeight="1">
+      <c r="B36" s="32" t="s">
+        <v>30</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="7"/>
@@ -2072,12 +2156,12 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
       <c r="L36" s="8"/>
-      <c r="M36" s="16"/>
+      <c r="M36" s="14"/>
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
       <c r="P36" s="10"/>
-      <c r="Q36" s="7"/>
-      <c r="R36" s="7"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
       <c r="U36" s="7"/>
@@ -2088,9 +2172,9 @@
       <c r="Z36" s="7"/>
       <c r="AA36" s="8"/>
     </row>
-    <row r="37" spans="2:27">
-      <c r="B37" s="20" t="s">
-        <v>32</v>
+    <row r="37" spans="2:27" ht="18" customHeight="1">
+      <c r="B37" s="32" t="s">
+        <v>31</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="7"/>
@@ -2102,13 +2186,13 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
       <c r="L37" s="8"/>
-      <c r="M37" s="16"/>
+      <c r="M37" s="14"/>
       <c r="N37" s="7"/>
       <c r="O37" s="7"/>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="10"/>
-      <c r="R37" s="10"/>
-      <c r="S37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
       <c r="T37" s="7"/>
       <c r="U37" s="7"/>
       <c r="V37" s="7"/>
@@ -2118,9 +2202,9 @@
       <c r="Z37" s="7"/>
       <c r="AA37" s="8"/>
     </row>
-    <row r="38" spans="2:27">
-      <c r="B38" s="20" t="s">
-        <v>33</v>
+    <row r="38" spans="2:27" ht="18" customHeight="1">
+      <c r="B38" s="32" t="s">
+        <v>32</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="7"/>
@@ -2132,25 +2216,25 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
       <c r="L38" s="8"/>
-      <c r="M38" s="16"/>
+      <c r="M38" s="14"/>
       <c r="N38" s="7"/>
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
-      <c r="Q38" s="7"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="7"/>
-      <c r="T38" s="7"/>
-      <c r="U38" s="10"/>
-      <c r="V38" s="10"/>
-      <c r="W38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
       <c r="X38" s="7"/>
       <c r="Y38" s="7"/>
       <c r="Z38" s="7"/>
       <c r="AA38" s="8"/>
     </row>
-    <row r="39" spans="2:27">
-      <c r="B39" s="20" t="s">
-        <v>34</v>
+    <row r="39" spans="2:27" ht="18" customHeight="1">
+      <c r="B39" s="32" t="s">
+        <v>33</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="7"/>
@@ -2162,25 +2246,25 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
       <c r="L39" s="8"/>
-      <c r="M39" s="16"/>
+      <c r="M39" s="14"/>
       <c r="N39" s="7"/>
       <c r="O39" s="7"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
       <c r="R39" s="7"/>
       <c r="S39" s="7"/>
-      <c r="T39" s="7"/>
-      <c r="U39" s="11"/>
-      <c r="V39" s="11"/>
-      <c r="W39" s="11"/>
-      <c r="X39" s="11"/>
-      <c r="Y39" s="11"/>
-      <c r="Z39" s="11"/>
-      <c r="AA39" s="12"/>
-    </row>
-    <row r="40" spans="2:27">
-      <c r="B40" s="20" t="s">
-        <v>35</v>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10"/>
+      <c r="W39" s="10"/>
+      <c r="X39" s="7"/>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="7"/>
+      <c r="AA39" s="8"/>
+    </row>
+    <row r="40" spans="2:27" ht="18" customHeight="1">
+      <c r="B40" s="32" t="s">
+        <v>34</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="7"/>
@@ -2192,25 +2276,25 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
       <c r="L40" s="8"/>
-      <c r="M40" s="16"/>
+      <c r="M40" s="14"/>
       <c r="N40" s="7"/>
       <c r="O40" s="7"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-      <c r="S40" s="10"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
       <c r="T40" s="7"/>
-      <c r="U40" s="7"/>
-      <c r="V40" s="7"/>
-      <c r="W40" s="7"/>
-      <c r="X40" s="7"/>
-      <c r="Y40" s="7"/>
-      <c r="Z40" s="7"/>
-      <c r="AA40" s="8"/>
-    </row>
-    <row r="41" spans="2:27">
-      <c r="B41" s="20" t="s">
-        <v>36</v>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
+      <c r="W40" s="10"/>
+      <c r="X40" s="10"/>
+      <c r="Y40" s="10"/>
+      <c r="Z40" s="10"/>
+      <c r="AA40" s="13"/>
+    </row>
+    <row r="41" spans="2:27" ht="18" customHeight="1">
+      <c r="B41" s="32" t="s">
+        <v>35</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="7"/>
@@ -2221,14 +2305,14 @@
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
-      <c r="L41" s="13"/>
-      <c r="M41" s="17"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="14"/>
       <c r="N41" s="7"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="7"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
       <c r="T41" s="7"/>
       <c r="U41" s="7"/>
       <c r="V41" s="7"/>
@@ -2238,9 +2322,9 @@
       <c r="Z41" s="7"/>
       <c r="AA41" s="8"/>
     </row>
-    <row r="42" spans="2:27">
-      <c r="B42" s="20" t="s">
-        <v>37</v>
+    <row r="42" spans="2:27" ht="18" customHeight="1">
+      <c r="B42" s="32" t="s">
+        <v>36</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="7"/>
@@ -2252,8 +2336,8 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
       <c r="L42" s="13"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="10"/>
+      <c r="M42" s="15"/>
+      <c r="N42" s="7"/>
       <c r="O42" s="7"/>
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
@@ -2268,9 +2352,9 @@
       <c r="Z42" s="7"/>
       <c r="AA42" s="8"/>
     </row>
-    <row r="43" spans="2:27">
-      <c r="B43" s="20" t="s">
-        <v>38</v>
+    <row r="43" spans="2:27" ht="18" customHeight="1">
+      <c r="B43" s="32" t="s">
+        <v>37</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="7"/>
@@ -2281,8 +2365,8 @@
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
-      <c r="L43" s="8"/>
-      <c r="M43" s="17"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="15"/>
       <c r="N43" s="10"/>
       <c r="O43" s="7"/>
       <c r="P43" s="7"/>
@@ -2298,9 +2382,9 @@
       <c r="Z43" s="7"/>
       <c r="AA43" s="8"/>
     </row>
-    <row r="44" spans="2:27">
-      <c r="B44" s="20" t="s">
-        <v>39</v>
+    <row r="44" spans="2:27" ht="18" customHeight="1">
+      <c r="B44" s="32" t="s">
+        <v>38</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="7"/>
@@ -2312,8 +2396,8 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
       <c r="L44" s="8"/>
-      <c r="M44" s="16"/>
-      <c r="N44" s="7"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="10"/>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7"/>
@@ -2321,16 +2405,16 @@
       <c r="S44" s="7"/>
       <c r="T44" s="7"/>
       <c r="U44" s="7"/>
-      <c r="V44" s="10"/>
-      <c r="W44" s="10"/>
-      <c r="X44" s="10"/>
+      <c r="V44" s="7"/>
+      <c r="W44" s="7"/>
+      <c r="X44" s="7"/>
       <c r="Y44" s="7"/>
       <c r="Z44" s="7"/>
       <c r="AA44" s="8"/>
     </row>
-    <row r="45" spans="2:27">
-      <c r="B45" s="20" t="s">
-        <v>40</v>
+    <row r="45" spans="2:27" ht="18" customHeight="1">
+      <c r="B45" s="32" t="s">
+        <v>39</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="7"/>
@@ -2342,7 +2426,7 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
       <c r="L45" s="8"/>
-      <c r="M45" s="16"/>
+      <c r="M45" s="14"/>
       <c r="N45" s="7"/>
       <c r="O45" s="7"/>
       <c r="P45" s="7"/>
@@ -2351,16 +2435,16 @@
       <c r="S45" s="7"/>
       <c r="T45" s="7"/>
       <c r="U45" s="7"/>
-      <c r="V45" s="7"/>
+      <c r="V45" s="10"/>
       <c r="W45" s="10"/>
       <c r="X45" s="10"/>
       <c r="Y45" s="7"/>
       <c r="Z45" s="7"/>
       <c r="AA45" s="8"/>
     </row>
-    <row r="46" spans="2:27">
-      <c r="B46" s="20" t="s">
-        <v>41</v>
+    <row r="46" spans="2:27" ht="18" customHeight="1">
+      <c r="B46" s="32" t="s">
+        <v>40</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="7"/>
@@ -2372,7 +2456,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
       <c r="L46" s="8"/>
-      <c r="M46" s="16"/>
+      <c r="M46" s="14"/>
       <c r="N46" s="7"/>
       <c r="O46" s="7"/>
       <c r="P46" s="7"/>
@@ -2384,13 +2468,13 @@
       <c r="V46" s="7"/>
       <c r="W46" s="10"/>
       <c r="X46" s="10"/>
-      <c r="Y46" s="10"/>
-      <c r="Z46" s="10"/>
-      <c r="AA46" s="13"/>
-    </row>
-    <row r="47" spans="2:27">
-      <c r="B47" s="20" t="s">
-        <v>42</v>
+      <c r="Y46" s="7"/>
+      <c r="Z46" s="7"/>
+      <c r="AA46" s="8"/>
+    </row>
+    <row r="47" spans="2:27" ht="18" customHeight="1">
+      <c r="B47" s="32" t="s">
+        <v>41</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="7"/>
@@ -2402,7 +2486,7 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
       <c r="L47" s="8"/>
-      <c r="M47" s="16"/>
+      <c r="M47" s="14"/>
       <c r="N47" s="7"/>
       <c r="O47" s="7"/>
       <c r="P47" s="7"/>
@@ -2412,15 +2496,15 @@
       <c r="T47" s="7"/>
       <c r="U47" s="7"/>
       <c r="V47" s="7"/>
-      <c r="W47" s="11"/>
-      <c r="X47" s="11"/>
-      <c r="Y47" s="11"/>
-      <c r="Z47" s="11"/>
-      <c r="AA47" s="12"/>
-    </row>
-    <row r="48" spans="2:27">
-      <c r="B48" s="20" t="s">
-        <v>43</v>
+      <c r="W47" s="10"/>
+      <c r="X47" s="10"/>
+      <c r="Y47" s="10"/>
+      <c r="Z47" s="10"/>
+      <c r="AA47" s="13"/>
+    </row>
+    <row r="48" spans="2:27" ht="18" customHeight="1">
+      <c r="B48" s="32" t="s">
+        <v>42</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="7"/>
@@ -2432,7 +2516,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
       <c r="L48" s="8"/>
-      <c r="M48" s="16"/>
+      <c r="M48" s="14"/>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
       <c r="P48" s="7"/>
@@ -2441,16 +2525,16 @@
       <c r="S48" s="7"/>
       <c r="T48" s="7"/>
       <c r="U48" s="7"/>
-      <c r="V48" s="10"/>
-      <c r="W48" s="10"/>
-      <c r="X48" s="10"/>
+      <c r="V48" s="7"/>
+      <c r="W48" s="29"/>
+      <c r="X48" s="29"/>
       <c r="Y48" s="10"/>
       <c r="Z48" s="10"/>
       <c r="AA48" s="13"/>
     </row>
-    <row r="49" spans="2:27">
-      <c r="B49" s="20" t="s">
-        <v>44</v>
+    <row r="49" spans="2:27" ht="18" customHeight="1">
+      <c r="B49" s="32" t="s">
+        <v>43</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="7"/>
@@ -2462,7 +2546,7 @@
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
       <c r="L49" s="8"/>
-      <c r="M49" s="16"/>
+      <c r="M49" s="14"/>
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
       <c r="P49" s="7"/>
@@ -2478,9 +2562,9 @@
       <c r="Z49" s="10"/>
       <c r="AA49" s="13"/>
     </row>
-    <row r="50" spans="2:27">
-      <c r="B50" s="20" t="s">
-        <v>45</v>
+    <row r="50" spans="2:27" ht="18" customHeight="1">
+      <c r="B50" s="32" t="s">
+        <v>44</v>
       </c>
       <c r="C50" s="9"/>
       <c r="D50" s="7"/>
@@ -2492,7 +2576,7 @@
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
       <c r="L50" s="8"/>
-      <c r="M50" s="16"/>
+      <c r="M50" s="14"/>
       <c r="N50" s="7"/>
       <c r="O50" s="7"/>
       <c r="P50" s="7"/>
@@ -2508,9 +2592,9 @@
       <c r="Z50" s="10"/>
       <c r="AA50" s="13"/>
     </row>
-    <row r="51" spans="2:27">
-      <c r="B51" s="20" t="s">
-        <v>50</v>
+    <row r="51" spans="2:27" ht="18" customHeight="1">
+      <c r="B51" s="32" t="s">
+        <v>45</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="7"/>
@@ -2522,7 +2606,7 @@
       <c r="J51" s="7"/>
       <c r="K51" s="7"/>
       <c r="L51" s="8"/>
-      <c r="M51" s="16"/>
+      <c r="M51" s="14"/>
       <c r="N51" s="7"/>
       <c r="O51" s="7"/>
       <c r="P51" s="7"/>
@@ -2538,9 +2622,9 @@
       <c r="Z51" s="10"/>
       <c r="AA51" s="13"/>
     </row>
-    <row r="52" spans="2:27">
-      <c r="B52" s="20" t="s">
-        <v>46</v>
+    <row r="52" spans="2:27" ht="18" customHeight="1">
+      <c r="B52" s="32" t="s">
+        <v>50</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="7"/>
@@ -2552,7 +2636,7 @@
       <c r="J52" s="7"/>
       <c r="K52" s="7"/>
       <c r="L52" s="8"/>
-      <c r="M52" s="16"/>
+      <c r="M52" s="14"/>
       <c r="N52" s="7"/>
       <c r="O52" s="7"/>
       <c r="P52" s="7"/>
@@ -2568,9 +2652,9 @@
       <c r="Z52" s="10"/>
       <c r="AA52" s="13"/>
     </row>
-    <row r="53" spans="2:27">
-      <c r="B53" s="20" t="s">
-        <v>47</v>
+    <row r="53" spans="2:27" ht="18" customHeight="1">
+      <c r="B53" s="32" t="s">
+        <v>46</v>
       </c>
       <c r="C53" s="9"/>
       <c r="D53" s="7"/>
@@ -2582,7 +2666,7 @@
       <c r="J53" s="7"/>
       <c r="K53" s="7"/>
       <c r="L53" s="8"/>
-      <c r="M53" s="16"/>
+      <c r="M53" s="14"/>
       <c r="N53" s="7"/>
       <c r="O53" s="7"/>
       <c r="P53" s="7"/>
@@ -2591,16 +2675,16 @@
       <c r="S53" s="7"/>
       <c r="T53" s="7"/>
       <c r="U53" s="7"/>
-      <c r="V53" s="7"/>
-      <c r="W53" s="7"/>
-      <c r="X53" s="11"/>
-      <c r="Y53" s="11"/>
-      <c r="Z53" s="11"/>
-      <c r="AA53" s="12"/>
-    </row>
-    <row r="54" spans="2:27">
-      <c r="B54" s="20" t="s">
-        <v>48</v>
+      <c r="V53" s="10"/>
+      <c r="W53" s="10"/>
+      <c r="X53" s="10"/>
+      <c r="Y53" s="10"/>
+      <c r="Z53" s="10"/>
+      <c r="AA53" s="13"/>
+    </row>
+    <row r="54" spans="2:27" ht="18" customHeight="1">
+      <c r="B54" s="32" t="s">
+        <v>47</v>
       </c>
       <c r="C54" s="9"/>
       <c r="D54" s="7"/>
@@ -2612,7 +2696,7 @@
       <c r="J54" s="7"/>
       <c r="K54" s="7"/>
       <c r="L54" s="8"/>
-      <c r="M54" s="16"/>
+      <c r="M54" s="14"/>
       <c r="N54" s="7"/>
       <c r="O54" s="7"/>
       <c r="P54" s="7"/>
@@ -2623,51 +2707,84 @@
       <c r="U54" s="7"/>
       <c r="V54" s="7"/>
       <c r="W54" s="7"/>
-      <c r="X54" s="7"/>
+      <c r="X54" s="11"/>
       <c r="Y54" s="11"/>
       <c r="Z54" s="11"/>
       <c r="AA54" s="12"/>
     </row>
-    <row r="55" spans="2:27">
-      <c r="B55" s="21" t="s">
+    <row r="55" spans="2:27" ht="18" customHeight="1">
+      <c r="B55" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="8"/>
+      <c r="M55" s="14"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7"/>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7"/>
+      <c r="S55" s="7"/>
+      <c r="T55" s="7"/>
+      <c r="U55" s="7"/>
+      <c r="V55" s="7"/>
+      <c r="W55" s="7"/>
+      <c r="X55" s="7"/>
+      <c r="Y55" s="11"/>
+      <c r="Z55" s="11"/>
+      <c r="AA55" s="12"/>
+    </row>
+    <row r="56" spans="2:27" ht="18" customHeight="1">
+      <c r="B56" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="22"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23"/>
-      <c r="F55" s="23"/>
-      <c r="G55" s="23"/>
-      <c r="H55" s="23"/>
-      <c r="I55" s="23"/>
-      <c r="J55" s="23"/>
-      <c r="K55" s="23"/>
-      <c r="L55" s="24"/>
-      <c r="M55" s="25"/>
-      <c r="N55" s="23"/>
-      <c r="O55" s="23"/>
-      <c r="P55" s="23"/>
-      <c r="Q55" s="23"/>
-      <c r="R55" s="23"/>
-      <c r="S55" s="23"/>
-      <c r="T55" s="23"/>
-      <c r="U55" s="23"/>
-      <c r="V55" s="23"/>
-      <c r="W55" s="23"/>
-      <c r="X55" s="23"/>
-      <c r="Y55" s="26"/>
-      <c r="Z55" s="26"/>
-      <c r="AA55" s="27"/>
-    </row>
-    <row r="56" spans="2:27">
-      <c r="B56" s="1"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="20"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="18"/>
+      <c r="Q56" s="18"/>
+      <c r="R56" s="18"/>
+      <c r="S56" s="18"/>
+      <c r="T56" s="18"/>
+      <c r="U56" s="18"/>
+      <c r="V56" s="18"/>
+      <c r="W56" s="18"/>
+      <c r="X56" s="18"/>
+      <c r="Y56" s="21"/>
+      <c r="Z56" s="21"/>
+      <c r="AA56" s="22"/>
     </row>
     <row r="57" spans="2:27">
       <c r="B57" s="1"/>
     </row>
+    <row r="58" spans="2:27">
+      <c r="B58" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="C4:L4"/>
     <mergeCell ref="M4:AA4"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="C5:AA5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>